<commit_message>
Subiendo generacion de reporte completo
</commit_message>
<xml_diff>
--- a/dias_semana.xlsx
+++ b/dias_semana.xlsx
@@ -460,7 +460,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -469,7 +469,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -479,7 +479,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -493,16 +493,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -512,7 +512,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -521,16 +521,16 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>240</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completanto funcionalidad de pagos pendientes
</commit_message>
<xml_diff>
--- a/dias_semana.xlsx
+++ b/dias_semana.xlsx
@@ -474,7 +474,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -488,7 +488,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>160</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3">
@@ -512,16 +512,16 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>80</v>
+        <v>240</v>
       </c>
     </row>
     <row r="4">
@@ -530,7 +530,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -540,7 +540,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>